<commit_message>
add xlsx 2 json
</commit_message>
<xml_diff>
--- a/xlsx/C1-测试.xlsx
+++ b/xlsx/C1-测试.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Obj-user" sheetId="1" r:id="rId1"/>
-    <sheet name="Tbl-city" sheetId="2" r:id="rId2"/>
-    <sheet name="Tbl-food" sheetId="3" r:id="rId3"/>
-    <sheet name="Enum-language" sheetId="4" r:id="rId4"/>
+    <sheet name="user" sheetId="1" r:id="rId1"/>
+    <sheet name="city" sheetId="2" r:id="rId2"/>
+    <sheet name="food" sheetId="3" r:id="rId3"/>
+    <sheet name="language" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -407,7 +407,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>测试表</v>
+        <v>##OBJ--用户表</v>
       </c>
     </row>
     <row r="2">
@@ -415,7 +415,7 @@
         <v>key</v>
       </c>
       <c r="B2" t="str">
-        <v>keyType</v>
+        <v>type</v>
       </c>
       <c r="C2" t="str">
         <v>value</v>
@@ -461,33 +461,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>测试lua数据表</v>
+        <v>##TBL--城市表</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>索引</v>
+        <v>id</v>
       </c>
       <c r="B2" t="str">
-        <v>城市名</v>
+        <v>cityName</v>
       </c>
       <c r="C2" t="str">
-        <v>省份</v>
+        <v>province</v>
       </c>
       <c r="D2" t="str">
-        <v>特产</v>
+        <v>food</v>
+      </c>
+      <c r="E2" t="str">
+        <v>regions</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>str</v>
+        <v>xid</v>
       </c>
       <c r="B3" t="str">
         <v>str</v>
@@ -498,19 +501,25 @@
       <c r="D3" t="str">
         <v>global::food</v>
       </c>
+      <c r="E3" t="str">
+        <v>list:str</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>xid</v>
+        <v>索引</v>
       </c>
       <c r="B4" t="str">
-        <v>cityName</v>
+        <v>城市名</v>
       </c>
       <c r="C4" t="str">
-        <v>province</v>
+        <v>省份</v>
       </c>
       <c r="D4" t="str">
-        <v>food</v>
+        <v>特产</v>
+      </c>
+      <c r="E4" t="str">
+        <v>行政区</v>
       </c>
     </row>
     <row r="5">
@@ -526,6 +535,9 @@
       <c r="D5" t="str">
         <v>1,2</v>
       </c>
+      <c r="E5" t="str">
+        <v>天河区,海珠区</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -540,10 +552,13 @@
       <c r="D6" t="str">
         <v>2</v>
       </c>
+      <c r="E6" t="str">
+        <v>西湖区,新建区</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -557,26 +572,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>内嵌表</v>
+        <v>##TBL--特产表</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>索引</v>
+        <v>id</v>
       </c>
       <c r="B2" t="str">
-        <v>食物名</v>
+        <v>name</v>
       </c>
       <c r="C2" t="str">
-        <v>类别</v>
+        <v>type</v>
       </c>
       <c r="D2" t="str">
-        <v>关联城市</v>
+        <v>city</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>num</v>
+        <v>xid</v>
       </c>
       <c r="B3" t="str">
         <v>str</v>
@@ -590,16 +605,16 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>xid</v>
+        <v>索引</v>
       </c>
       <c r="B4" t="str">
-        <v>name</v>
+        <v>食物名</v>
       </c>
       <c r="C4" t="str">
-        <v>type</v>
+        <v>类别</v>
       </c>
       <c r="D4" t="str">
-        <v>city</v>
+        <v>关联城市</v>
       </c>
     </row>
     <row r="5">
@@ -646,7 +661,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>测试lua枚举</v>
+        <v>##ENUM--语言表</v>
       </c>
     </row>
     <row r="2">

</xml_diff>